<commit_message>
Abschluss Zinsberechnung, Anfang: refactor Buchungen
</commit_message>
<xml_diff>
--- a/DOCS/ZinsBerechnung.xlsx
+++ b/DOCS/ZinsBerechnung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\home\dev\DKV2\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\qt-dev\home\dev\DKV2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{85403EF9-5801-4C28-BD95-450183D2C397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BB34D25B-A1B7-47CB-AB32-E8A23D2838BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10095" yWindow="2595" windowWidth="22815" windowHeight="11325" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zinseszins" sheetId="3" r:id="rId1"/>
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -218,7 +218,7 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -539,10 +539,10 @@
   <dimension ref="A2:BI16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AD10" sqref="AD10"/>
+      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:61" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -662,7 +662,9 @@
       <c r="AE5" s="15" t="d">
         <v>2015-12-31</v>
       </c>
-      <c r="AF5" s="14"/>
+      <c r="AF5" s="15" t="d">
+        <v>2015-01-01</v>
+      </c>
       <c r="AG5" s="14"/>
       <c r="AH5" s="14"/>
       <c r="AI5" s="14"/>
@@ -785,7 +787,9 @@
       <c r="AE6" s="15" t="d">
         <v>2024-02-29</v>
       </c>
-      <c r="AF6" s="14"/>
+      <c r="AF6" s="15" t="d">
+        <v>2025-01-01</v>
+      </c>
       <c r="AG6" s="14"/>
       <c r="AH6" s="14"/>
       <c r="AI6" s="14"/>
@@ -938,7 +942,7 @@
       </c>
       <c r="AF7" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>359</v>
       </c>
       <c r="AG7" s="17">
         <f t="shared" si="0"/>
@@ -1062,239 +1066,239 @@
         <v>16</v>
       </c>
       <c r="C8" s="16">
-        <f>ROUND(C$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" ref="C8:AH8" si="1">ROUND(C$7*ZINSSATZ*WERT/360,2)</f>
         <v>0.81</v>
       </c>
       <c r="D8" s="16">
-        <f>ROUND(D$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0.81</v>
       </c>
       <c r="E8" s="16">
-        <f>ROUND(E$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>9.17</v>
       </c>
       <c r="F8" s="16">
-        <f>ROUND(F$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8" s="16">
-        <f>ROUND(G$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <f>ROUND(H$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>9.17</v>
       </c>
       <c r="I8" s="16">
-        <f>ROUND(I$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>9.17</v>
       </c>
       <c r="J8" s="16">
-        <f>ROUND(J$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>8.36</v>
       </c>
       <c r="K8" s="16">
-        <f>ROUND(K$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="L8" s="16">
-        <f>ROUND(L$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>6.67</v>
       </c>
       <c r="M8" s="16">
-        <f>ROUND(M$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>5.83</v>
       </c>
       <c r="N8" s="16">
-        <f>ROUND(N$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="O8" s="16">
-        <f>ROUND(O$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>4.17</v>
       </c>
       <c r="P8" s="16">
-        <f>ROUND(P$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>3.33</v>
       </c>
       <c r="Q8" s="16">
-        <f>ROUND(Q$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="R8" s="16">
-        <f>ROUND(R$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>1.67</v>
       </c>
       <c r="S8" s="16">
-        <f>ROUND(S$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0.83</v>
       </c>
       <c r="T8" s="16">
-        <f>ROUND(T$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U8" s="16">
-        <f>ROUND(U$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V8" s="16">
-        <f>ROUND(V$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W8" s="16">
-        <f>ROUND(W$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X8" s="16">
-        <f>ROUND(X$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y8" s="16">
-        <f>ROUND(Y$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z8" s="16">
-        <f>ROUND(Z$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AA8" s="16">
-        <f>ROUND(AA$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB8" s="16">
-        <f>ROUND(AB$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC8" s="16">
-        <f>ROUND(AC$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD8" s="16">
-        <f>ROUND(AD$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE8" s="16">
-        <f>ROUND(AE$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF8" s="16">
-        <f>ROUND(AF$7*ZINSSATZ*WERT/360,2)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9.9700000000000006</v>
       </c>
       <c r="AG8" s="16">
-        <f>ROUND(AG$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH8" s="16">
-        <f>ROUND(AH$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI8" s="16">
-        <f>ROUND(AI$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" ref="AI8:BI8" si="2">ROUND(AI$7*ZINSSATZ*WERT/360,2)</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="16">
-        <f>ROUND(AJ$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK8" s="16">
-        <f>ROUND(AK$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL8" s="16">
-        <f>ROUND(AL$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM8" s="16">
-        <f>ROUND(AM$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AN8" s="16">
-        <f>ROUND(AN$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AO8" s="16">
-        <f>ROUND(AO$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AP8" s="16">
-        <f>ROUND(AP$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AQ8" s="16">
-        <f>ROUND(AQ$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AR8" s="16">
-        <f>ROUND(AR$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS8" s="16">
-        <f>ROUND(AS$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AT8" s="16">
-        <f>ROUND(AT$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AU8" s="16">
-        <f>ROUND(AU$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AV8" s="16">
-        <f>ROUND(AV$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AW8" s="16">
-        <f>ROUND(AW$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AX8" s="16">
-        <f>ROUND(AX$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AY8" s="16">
-        <f>ROUND(AY$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AZ8" s="16">
-        <f>ROUND(AZ$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BA8" s="16">
-        <f>ROUND(BA$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BB8" s="16">
-        <f>ROUND(BB$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BC8" s="16">
-        <f>ROUND(BC$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BD8" s="16">
-        <f>ROUND(BD$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BE8" s="16">
-        <f>ROUND(BE$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BF8" s="16">
-        <f>ROUND(BF$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BG8" s="16">
-        <f>ROUND(BG$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BH8" s="16">
-        <f>ROUND(BH$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BI8" s="16">
-        <f>ROUND(BI$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1307,235 +1311,235 @@
         <v>1</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" ref="D9:BI9" si="1">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),MAX(YEAR(D$6)-YEAR(D$5)-1,0),0)</f>
+        <f t="shared" ref="D9:BI9" si="3">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),MAX(YEAR(D$6)-YEAR(D$5)-1,0),0)</f>
         <v>1</v>
       </c>
       <c r="E9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="V9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Y9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Z9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="AA9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="AB9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="AC9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="AD9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AE9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="AF9" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
       <c r="AG9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AL9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AN9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AR9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AS9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AT9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AU9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AV9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AW9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AX9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AY9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AZ9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BA9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BB9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BC9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BE9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BG9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BH9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BI9" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1544,239 +1548,239 @@
         <v>17</v>
       </c>
       <c r="C10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-C$8+(WERT+C$8)*(1+ZINSSATZ)^C$9,2)</f>
+        <f t="shared" ref="C10:AH10" si="4" xml:space="preserve"> ROUND(-WERT-C$8+(WERT+C$8)*(1+ZINSSATZ)^C$9,2)</f>
         <v>10.08</v>
       </c>
       <c r="D10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-D$8+(WERT+D$8)*(1+ZINSSATZ)^D$9,2)</f>
+        <f t="shared" si="4"/>
         <v>10.08</v>
       </c>
       <c r="E10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-E$8+(WERT+E$8)*(1+ZINSSATZ)^E$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-F$8+(WERT+F$8)*(1+ZINSSATZ)^F$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-G$8+(WERT+G$8)*(1+ZINSSATZ)^G$9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-H$8+(WERT+H$8)*(1+ZINSSATZ)^H$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-I$8+(WERT+I$8)*(1+ZINSSATZ)^I$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-J$8+(WERT+J$8)*(1+ZINSSATZ)^J$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-K$8+(WERT+K$8)*(1+ZINSSATZ)^K$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-L$8+(WERT+L$8)*(1+ZINSSATZ)^L$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-M$8+(WERT+M$8)*(1+ZINSSATZ)^M$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-N$8+(WERT+N$8)*(1+ZINSSATZ)^N$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-O$8+(WERT+O$8)*(1+ZINSSATZ)^O$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-P$8+(WERT+P$8)*(1+ZINSSATZ)^P$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-Q$8+(WERT+Q$8)*(1+ZINSSATZ)^Q$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-R$8+(WERT+R$8)*(1+ZINSSATZ)^R$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-S$8+(WERT+S$8)*(1+ZINSSATZ)^S$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-T$8+(WERT+T$8)*(1+ZINSSATZ)^T$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-U$8+(WERT+U$8)*(1+ZINSSATZ)^U$9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="V10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-V$8+(WERT+V$8)*(1+ZINSSATZ)^V$9,2)</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="W10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-W$8+(WERT+W$8)*(1+ZINSSATZ)^W$9,2)</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="X10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-X$8+(WERT+X$8)*(1+ZINSSATZ)^X$9,2)</f>
+        <f t="shared" si="4"/>
         <v>33.1</v>
       </c>
       <c r="Y10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-Y$8+(WERT+Y$8)*(1+ZINSSATZ)^Y$9,2)</f>
+        <f t="shared" si="4"/>
         <v>33.1</v>
       </c>
       <c r="Z10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-Z$8+(WERT+Z$8)*(1+ZINSSATZ)^Z$9,2)</f>
+        <f t="shared" si="4"/>
         <v>34.76</v>
       </c>
       <c r="AA10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AA$8+(WERT+AA$8)*(1+ZINSSATZ)^AA$9,2)</f>
+        <f t="shared" si="4"/>
         <v>46.41</v>
       </c>
       <c r="AB10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AB$8+(WERT+AB$8)*(1+ZINSSATZ)^AB$9,2)</f>
+        <f t="shared" si="4"/>
         <v>46.41</v>
       </c>
       <c r="AC10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AC$8+(WERT+AC$8)*(1+ZINSSATZ)^AC$9,2)</f>
+        <f t="shared" si="4"/>
         <v>61.05</v>
       </c>
       <c r="AD10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AD$8+(WERT+AD$8)*(1+ZINSSATZ)^AD$9,2)</f>
+        <f t="shared" si="4"/>
         <v>114.36</v>
       </c>
       <c r="AE10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AE$8+(WERT+AE$8)*(1+ZINSSATZ)^AE$9,2)</f>
+        <f t="shared" si="4"/>
         <v>114.36</v>
       </c>
       <c r="AF10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AF$8+(WERT+AF$8)*(1+ZINSSATZ)^AF$9,2)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>149.33000000000001</v>
       </c>
       <c r="AG10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AG$8+(WERT+AG$8)*(1+ZINSSATZ)^AG$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AH$8+(WERT+AH$8)*(1+ZINSSATZ)^AH$9,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AI$8+(WERT+AI$8)*(1+ZINSSATZ)^AI$9,2)</f>
+        <f t="shared" ref="AI10:BI10" si="5" xml:space="preserve"> ROUND(-WERT-AI$8+(WERT+AI$8)*(1+ZINSSATZ)^AI$9,2)</f>
         <v>0</v>
       </c>
       <c r="AJ10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AJ$8+(WERT+AJ$8)*(1+ZINSSATZ)^AJ$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AK$8+(WERT+AK$8)*(1+ZINSSATZ)^AK$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AL10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AL$8+(WERT+AL$8)*(1+ZINSSATZ)^AL$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AM$8+(WERT+AM$8)*(1+ZINSSATZ)^AM$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AN10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AN$8+(WERT+AN$8)*(1+ZINSSATZ)^AN$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AO$8+(WERT+AO$8)*(1+ZINSSATZ)^AO$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AP10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AP$8+(WERT+AP$8)*(1+ZINSSATZ)^AP$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AQ10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AQ$8+(WERT+AQ$8)*(1+ZINSSATZ)^AQ$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AR10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AR$8+(WERT+AR$8)*(1+ZINSSATZ)^AR$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AS10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AS$8+(WERT+AS$8)*(1+ZINSSATZ)^AS$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AT10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AT$8+(WERT+AT$8)*(1+ZINSSATZ)^AT$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AU10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AU$8+(WERT+AU$8)*(1+ZINSSATZ)^AU$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AV10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AV$8+(WERT+AV$8)*(1+ZINSSATZ)^AV$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AW10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AW$8+(WERT+AW$8)*(1+ZINSSATZ)^AW$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AX10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AX$8+(WERT+AX$8)*(1+ZINSSATZ)^AX$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AY10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AY$8+(WERT+AY$8)*(1+ZINSSATZ)^AY$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AZ10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-AZ$8+(WERT+AZ$8)*(1+ZINSSATZ)^AZ$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BA10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BA$8+(WERT+BA$8)*(1+ZINSSATZ)^BA$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BB10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BB$8+(WERT+BB$8)*(1+ZINSSATZ)^BB$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BC10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BC$8+(WERT+BC$8)*(1+ZINSSATZ)^BC$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BD10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BD$8+(WERT+BD$8)*(1+ZINSSATZ)^BD$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BE10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BE$8+(WERT+BE$8)*(1+ZINSSATZ)^BE$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BF10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BF$8+(WERT+BF$8)*(1+ZINSSATZ)^BF$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BG10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BG$8+(WERT+BG$8)*(1+ZINSSATZ)^BG$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BH10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BH$8+(WERT+BH$8)*(1+ZINSSATZ)^BH$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BI10" s="12">
-        <f xml:space="preserve"> ROUND(-WERT-BI$8+(WERT+BI$8)*(1+ZINSSATZ)^BI$9,2)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1785,239 +1789,239 @@
         <v>18</v>
       </c>
       <c r="C11" s="12">
-        <f>ROUND(C$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" ref="C11:AH11" si="6">ROUND(C$9*WERT*ZINSSATZ,2)</f>
         <v>10</v>
       </c>
       <c r="D11" s="12">
-        <f>ROUND(D$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="E11" s="12">
-        <f>ROUND(E$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F11" s="12">
-        <f>ROUND(F$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G11" s="12">
-        <f>ROUND(G$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="H11" s="12">
-        <f>ROUND(H$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11" s="12">
-        <f>ROUND(I$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J11" s="12">
-        <f>ROUND(J$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K11" s="12">
-        <f>ROUND(K$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L11" s="12">
-        <f>ROUND(L$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M11" s="12">
-        <f>ROUND(M$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N11" s="12">
-        <f>ROUND(N$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O11" s="12">
-        <f>ROUND(O$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P11" s="12">
-        <f>ROUND(P$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q11" s="12">
-        <f>ROUND(Q$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R11" s="12">
-        <f>ROUND(R$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S11" s="12">
-        <f>ROUND(S$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T11" s="12">
-        <f>ROUND(T$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U11" s="12">
-        <f>ROUND(U$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="V11" s="12">
-        <f>ROUND(V$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="W11" s="12">
-        <f>ROUND(W$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="X11" s="12">
-        <f>ROUND(X$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="Y11" s="12">
-        <f>ROUND(Y$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="Z11" s="12">
-        <f>ROUND(Z$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="AA11" s="12">
-        <f>ROUND(AA$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="AB11" s="12">
-        <f>ROUND(AB$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="AC11" s="12">
-        <f>ROUND(AC$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="AD11" s="12">
-        <f>ROUND(AD$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="AE11" s="12">
-        <f>ROUND(AE$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="AF11" s="12">
-        <f>ROUND(AF$9*WERT*ZINSSATZ,2)</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>90</v>
       </c>
       <c r="AG11" s="12">
-        <f>ROUND(AG$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AH11" s="12">
-        <f>ROUND(AH$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI11" s="12">
-        <f>ROUND(AI$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" ref="AI11:BI11" si="7">ROUND(AI$9*WERT*ZINSSATZ,2)</f>
         <v>0</v>
       </c>
       <c r="AJ11" s="12">
-        <f>ROUND(AJ$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AK11" s="12">
-        <f>ROUND(AK$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AL11" s="12">
-        <f>ROUND(AL$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AM11" s="12">
-        <f>ROUND(AM$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AN11" s="12">
-        <f>ROUND(AN$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AO11" s="12">
-        <f>ROUND(AO$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AP11" s="12">
-        <f>ROUND(AP$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ11" s="12">
-        <f>ROUND(AQ$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AR11" s="12">
-        <f>ROUND(AR$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AS11" s="12">
-        <f>ROUND(AS$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AT11" s="12">
-        <f>ROUND(AT$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AU11" s="12">
-        <f>ROUND(AU$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AV11" s="12">
-        <f>ROUND(AV$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW11" s="12">
-        <f>ROUND(AW$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AX11" s="12">
-        <f>ROUND(AX$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AY11" s="12">
-        <f>ROUND(AY$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AZ11" s="12">
-        <f>ROUND(AZ$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BA11" s="12">
-        <f>ROUND(BA$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BB11" s="12">
-        <f>ROUND(BB$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BC11" s="12">
-        <f>ROUND(BC$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BD11" s="12">
-        <f>ROUND(BD$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BE11" s="12">
-        <f>ROUND(BE$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BF11" s="12">
-        <f>ROUND(BF$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BG11" s="12">
-        <f>ROUND(BG$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BH11" s="12">
-        <f>ROUND(BH$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="BI11" s="12">
-        <f>ROUND(BI$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2030,235 +2034,235 @@
         <v>30</v>
       </c>
       <c r="D12" s="17">
-        <f t="shared" ref="D12:BI12" si="2">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
+        <f t="shared" ref="D12:BI12" si="8">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="E12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>61</v>
       </c>
       <c r="F12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>360</v>
       </c>
       <c r="G12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="H12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
       <c r="I12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
       <c r="J12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>61</v>
       </c>
       <c r="K12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="L12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>121</v>
       </c>
       <c r="M12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>151</v>
       </c>
       <c r="N12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>181</v>
       </c>
       <c r="O12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>211</v>
       </c>
       <c r="P12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>241</v>
       </c>
       <c r="Q12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>271</v>
       </c>
       <c r="R12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>301</v>
       </c>
       <c r="S12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>331</v>
       </c>
       <c r="T12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="U12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="V12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="W12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="X12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Y12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="Z12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>360</v>
       </c>
       <c r="AA12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AB12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="AC12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AD12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
       <c r="AE12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
       <c r="AF12" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="AG12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AK12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AL12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AM12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AN12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AP12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AQ12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AS12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AT12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AU12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AV12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AY12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AZ12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BA12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BC12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BD12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BE12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BF12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BG12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BH12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BI12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -2267,239 +2271,239 @@
         <v>19</v>
       </c>
       <c r="C13" s="16">
-        <f>ROUND((WERT+C$8+C$10)*C$12/360*ZINSSATZ,2)</f>
+        <f t="shared" ref="C13:AH13" si="9">ROUND((WERT+C$8+C$10)*C$12/360*ZINSSATZ,2)</f>
         <v>0.92</v>
       </c>
       <c r="D13" s="16">
-        <f>ROUND((WERT+D$8+D$10)*D$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.03</v>
       </c>
       <c r="E13" s="16">
-        <f>ROUND((WERT+E$8+E$10)*E$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>1.85</v>
       </c>
       <c r="F13" s="16">
-        <f>ROUND((WERT+F$8+F$10)*F$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="G13" s="16">
-        <f>ROUND((WERT+G$8+G$10)*G$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.92</v>
       </c>
       <c r="H13" s="16">
-        <f>ROUND((WERT+H$8+H$10)*H$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>1.76</v>
       </c>
       <c r="I13" s="16">
-        <f>ROUND((WERT+I$8+I$10)*I$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.94</v>
       </c>
       <c r="J13" s="16">
-        <f>ROUND((WERT+J$8+J$10)*J$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>1.84</v>
       </c>
       <c r="K13" s="16">
-        <f>ROUND((WERT+K$8+K$10)*K$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>2.72</v>
       </c>
       <c r="L13" s="16">
-        <f>ROUND((WERT+L$8+L$10)*L$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>3.59</v>
       </c>
       <c r="M13" s="16">
-        <f>ROUND((WERT+M$8+M$10)*M$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>4.4400000000000004</v>
       </c>
       <c r="N13" s="16">
-        <f>ROUND((WERT+N$8+N$10)*N$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>5.28</v>
       </c>
       <c r="O13" s="16">
-        <f>ROUND((WERT+O$8+O$10)*O$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>6.11</v>
       </c>
       <c r="P13" s="16">
-        <f>ROUND((WERT+P$8+P$10)*P$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>6.92</v>
       </c>
       <c r="Q13" s="16">
-        <f>ROUND((WERT+Q$8+Q$10)*Q$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>7.72</v>
       </c>
       <c r="R13" s="16">
-        <f>ROUND((WERT+R$8+R$10)*R$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>8.5</v>
       </c>
       <c r="S13" s="16">
-        <f>ROUND((WERT+S$8+S$10)*S$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>9.27</v>
       </c>
       <c r="T13" s="16">
-        <f>ROUND((WERT+T$8+T$10)*T$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="U13" s="16">
-        <f>ROUND((WERT+U$8+U$10)*U$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="V13" s="16">
-        <f>ROUND((WERT+V$8+V$10)*V$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.03</v>
       </c>
       <c r="W13" s="16">
-        <f>ROUND((WERT+W$8+W$10)*W$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>6.05</v>
       </c>
       <c r="X13" s="16">
-        <f>ROUND((WERT+X$8+X$10)*X$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.04</v>
       </c>
       <c r="Y13" s="16">
-        <f>ROUND((WERT+Y$8+Y$10)*Y$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>6.66</v>
       </c>
       <c r="Z13" s="16">
-        <f>ROUND((WERT+Z$8+Z$10)*Z$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>13.98</v>
       </c>
       <c r="AA13" s="16">
-        <f>ROUND((WERT+AA$8+AA$10)*AA$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.04</v>
       </c>
       <c r="AB13" s="16">
-        <f>ROUND((WERT+AB$8+AB$10)*AB$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>7.32</v>
       </c>
       <c r="AC13" s="16">
-        <f>ROUND((WERT+AC$8+AC$10)*AC$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0.04</v>
       </c>
       <c r="AD13" s="16">
-        <f>ROUND((WERT+AD$8+AD$10)*AD$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>3.45</v>
       </c>
       <c r="AE13" s="16">
-        <f>ROUND((WERT+AE$8+AE$10)*AE$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>3.51</v>
       </c>
       <c r="AF13" s="16">
-        <f>ROUND((WERT+AF$8+AF$10)*AF$12/360*ZINSSATZ,2)</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AG13" s="16">
-        <f>ROUND((WERT+AG$8+AG$10)*AG$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH13" s="16">
-        <f>ROUND((WERT+AH$8+AH$10)*AH$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI13" s="16">
-        <f>ROUND((WERT+AI$8+AI$10)*AI$12/360*ZINSSATZ,2)</f>
+        <f t="shared" ref="AI13:BI13" si="10">ROUND((WERT+AI$8+AI$10)*AI$12/360*ZINSSATZ,2)</f>
         <v>0</v>
       </c>
       <c r="AJ13" s="16">
-        <f>ROUND((WERT+AJ$8+AJ$10)*AJ$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK13" s="16">
-        <f>ROUND((WERT+AK$8+AK$10)*AK$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL13" s="16">
-        <f>ROUND((WERT+AL$8+AL$10)*AL$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AM13" s="16">
-        <f>ROUND((WERT+AM$8+AM$10)*AM$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AN13" s="16">
-        <f>ROUND((WERT+AN$8+AN$10)*AN$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AO13" s="16">
-        <f>ROUND((WERT+AO$8+AO$10)*AO$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AP13" s="16">
-        <f>ROUND((WERT+AP$8+AP$10)*AP$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AQ13" s="16">
-        <f>ROUND((WERT+AQ$8+AQ$10)*AQ$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AR13" s="16">
-        <f>ROUND((WERT+AR$8+AR$10)*AR$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AS13" s="16">
-        <f>ROUND((WERT+AS$8+AS$10)*AS$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT13" s="16">
-        <f>ROUND((WERT+AT$8+AT$10)*AT$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AU13" s="16">
-        <f>ROUND((WERT+AU$8+AU$10)*AU$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AV13" s="16">
-        <f>ROUND((WERT+AV$8+AV$10)*AV$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AW13" s="16">
-        <f>ROUND((WERT+AW$8+AW$10)*AW$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AX13" s="16">
-        <f>ROUND((WERT+AX$8+AX$10)*AX$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AY13" s="16">
-        <f>ROUND((WERT+AY$8+AY$10)*AY$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AZ13" s="16">
-        <f>ROUND((WERT+AZ$8+AZ$10)*AZ$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BA13" s="16">
-        <f>ROUND((WERT+BA$8+BA$10)*BA$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BB13" s="16">
-        <f>ROUND((WERT+BB$8+BB$10)*BB$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BC13" s="16">
-        <f>ROUND((WERT+BC$8+BC$10)*BC$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BD13" s="16">
-        <f>ROUND((WERT+BD$8+BD$10)*BD$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BE13" s="16">
-        <f>ROUND((WERT+BE$8+BE$10)*BE$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BF13" s="16">
-        <f>ROUND((WERT+BF$8+BF$10)*BF$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BG13" s="16">
-        <f>ROUND((WERT+BG$8+BG$10)*BG$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BH13" s="16">
-        <f>ROUND((WERT+BH$8+BH$10)*BH$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BI13" s="16">
-        <f>ROUND((WERT+BI$8+BI$10)*BI$12/360*ZINSSATZ,2)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -2508,239 +2512,239 @@
         <v>20</v>
       </c>
       <c r="C14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*C$12/360,2)</f>
+        <f t="shared" ref="C14:AH14" si="11">ROUND(WERT*ZINSSATZ*C$12/360,2)</f>
         <v>0.83</v>
       </c>
       <c r="D14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*D$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="E14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*E$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>1.69</v>
       </c>
       <c r="F14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*F$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="G14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*G$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.83</v>
       </c>
       <c r="H14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*H$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>1.61</v>
       </c>
       <c r="I14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*I$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.86</v>
       </c>
       <c r="J14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*J$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>1.69</v>
       </c>
       <c r="K14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*K$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>2.5299999999999998</v>
       </c>
       <c r="L14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*L$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>3.36</v>
       </c>
       <c r="M14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*M$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>4.1900000000000004</v>
       </c>
       <c r="N14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*N$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5.03</v>
       </c>
       <c r="O14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*O$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5.86</v>
       </c>
       <c r="P14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*P$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>6.69</v>
       </c>
       <c r="Q14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*Q$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>7.53</v>
       </c>
       <c r="R14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*R$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>8.36</v>
       </c>
       <c r="S14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*S$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>9.19</v>
       </c>
       <c r="T14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*T$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="U14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*U$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="V14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*V$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="W14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*W$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="X14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*X$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="Y14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*Y$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="Z14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*Z$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="AA14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AA$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="AB14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AB$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AC14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AC$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="AD14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AD$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>1.61</v>
       </c>
       <c r="AE14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AE$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>1.64</v>
       </c>
       <c r="AF14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AF$12/360,2)</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.03</v>
       </c>
       <c r="AG14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AG$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AH14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AH$12/360,2)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AI14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AI$12/360,2)</f>
+        <f t="shared" ref="AI14:BI14" si="12">ROUND(WERT*ZINSSATZ*AI$12/360,2)</f>
         <v>0</v>
       </c>
       <c r="AJ14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AJ$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AK$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AL14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AL$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AM14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AM$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AN14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AN$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AO14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AO$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AP14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AP$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AQ14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AQ$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AR14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AR$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AS14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AS$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AT14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AT$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AU14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AU$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AV$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AW14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AW$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AX14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AX$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AY14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AY$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AZ14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*AZ$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BA14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BA$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BB$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BC14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BC$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BD14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BD$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BE14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BE$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BF14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BF$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BG14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BG$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BH14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BH$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BI14" s="16">
-        <f>ROUND(WERT*ZINSSATZ*BI$12/360,2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -2756,235 +2760,235 @@
         <v>11.81</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" ref="D15:BI15" si="3">ROUND(D$8+D$10+D$13,2)</f>
+        <f t="shared" ref="D15:BI15" si="13">ROUND(D$8+D$10+D$13,2)</f>
         <v>10.92</v>
       </c>
       <c r="E15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>11.02</v>
       </c>
       <c r="F15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.92</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.93</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.11</v>
       </c>
       <c r="J15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.199999999999999</v>
       </c>
       <c r="K15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.220000000000001</v>
       </c>
       <c r="L15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.26</v>
       </c>
       <c r="M15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.27</v>
       </c>
       <c r="N15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.28</v>
       </c>
       <c r="O15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.28</v>
       </c>
       <c r="P15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.25</v>
       </c>
       <c r="Q15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.220000000000001</v>
       </c>
       <c r="R15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.17</v>
       </c>
       <c r="S15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>10.1</v>
       </c>
       <c r="T15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="U15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>15.5</v>
       </c>
       <c r="V15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>21.03</v>
       </c>
       <c r="W15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>27.05</v>
       </c>
       <c r="X15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>33.14</v>
       </c>
       <c r="Y15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>39.76</v>
       </c>
       <c r="Z15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>53.74</v>
       </c>
       <c r="AA15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>46.45</v>
       </c>
       <c r="AB15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>53.73</v>
       </c>
       <c r="AC15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>61.09</v>
       </c>
       <c r="AD15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>117.81</v>
       </c>
       <c r="AE15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>117.87</v>
       </c>
       <c r="AF15" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>159.37</v>
       </c>
       <c r="AG15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AH15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AK15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AN15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AO15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AP15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AQ15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AR15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AS15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AT15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AU15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AV15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AX15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AY15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AZ15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BA15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BB15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BC15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BD15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BE15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BF15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BG15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BH15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="BI15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -2997,235 +3001,235 @@
         <v>11.64</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" ref="D16:BI16" si="4">ROUND(D$8+D$11+D$14,2)</f>
+        <f t="shared" ref="D16:BI16" si="14">ROUND(D$8+D$11+D$14,2)</f>
         <v>10.84</v>
       </c>
       <c r="E16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.86</v>
       </c>
       <c r="F16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="G16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.83</v>
       </c>
       <c r="H16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.78</v>
       </c>
       <c r="I16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="J16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.050000000000001</v>
       </c>
       <c r="K16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="L16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="M16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.02</v>
       </c>
       <c r="N16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="O16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="P16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.02</v>
       </c>
       <c r="Q16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="R16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.029999999999999</v>
       </c>
       <c r="S16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>10.02</v>
       </c>
       <c r="T16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="U16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="V16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>20.03</v>
       </c>
       <c r="W16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="X16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>30.03</v>
       </c>
       <c r="Y16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>35</v>
       </c>
       <c r="Z16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>45</v>
       </c>
       <c r="AA16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>40.03</v>
       </c>
       <c r="AB16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>45</v>
       </c>
       <c r="AC16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>50.03</v>
       </c>
       <c r="AD16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>81.61</v>
       </c>
       <c r="AE16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>81.64</v>
       </c>
       <c r="AF16" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>100</v>
       </c>
       <c r="AG16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AI16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AK16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AL16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AN16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AO16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AP16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AQ16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AR16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AS16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AT16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AU16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AV16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AW16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AX16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AY16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AZ16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BA16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BB16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BC16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BD16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BE16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BF16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BG16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BH16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BI16" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Zinsberechnung: Korrektur: Vertrag innerhalb eines Jahres
</commit_message>
<xml_diff>
--- a/DOCS/ZinsBerechnung.xlsx
+++ b/DOCS/ZinsBerechnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\qt-dev\home\dev\DKV2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BB34D25B-A1B7-47CB-AB32-E8A23D2838BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0A702E37-44F8-47D0-A9BA-6D58917473C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
+    <workbookView xWindow="8970" yWindow="765" windowWidth="18810" windowHeight="14055" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zinseszins" sheetId="3" r:id="rId1"/>
@@ -536,13 +536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36E29AA-5770-4214-8700-B8EC11840B55}">
-  <dimension ref="A2:BI16"/>
+  <dimension ref="A2:BI19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AG5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
+      <selection pane="bottomRight" activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:61" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -665,12 +665,24 @@
       <c r="AF5" s="15" t="d">
         <v>2015-01-01</v>
       </c>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
+      <c r="AG5" s="15" t="d">
+        <v>2019-01-03</v>
+      </c>
+      <c r="AH5" s="15" t="d">
+        <v>2018-01-31</v>
+      </c>
+      <c r="AI5" s="15" t="d">
+        <v>2016-01-15</v>
+      </c>
+      <c r="AJ5" s="15" t="d">
+        <v>2016-01-15</v>
+      </c>
+      <c r="AK5" s="15" t="d">
+        <v>2014-01-05</v>
+      </c>
+      <c r="AL5" s="15" t="d">
+        <v>2014-06-01</v>
+      </c>
       <c r="AM5" s="14"/>
       <c r="AN5" s="14"/>
       <c r="AO5" s="14"/>
@@ -790,12 +802,24 @@
       <c r="AF6" s="15" t="d">
         <v>2025-01-01</v>
       </c>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
+      <c r="AG6" s="15" t="d">
+        <v>2019-11-04</v>
+      </c>
+      <c r="AH6" s="15" t="d">
+        <v>2018-11-30</v>
+      </c>
+      <c r="AI6" s="15" t="d">
+        <v>2016-02-29</v>
+      </c>
+      <c r="AJ6" s="15" t="d">
+        <v>2016-03-01</v>
+      </c>
+      <c r="AK6" s="15" t="d">
+        <v>2014-01-10</v>
+      </c>
+      <c r="AL6" s="15" t="d">
+        <v>2014-12-31</v>
+      </c>
       <c r="AM6" s="14"/>
       <c r="AN6" s="14"/>
       <c r="AO6" s="14"/>
@@ -825,11 +849,11 @@
         <v>11</v>
       </c>
       <c r="C7" s="17">
-        <f>IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),DAYS360(C$5,DATE(YEAR(C$5),12,31), TRUE),0)</f>
+        <f t="shared" ref="C7:AF7" si="0">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""), IF(YEAR(C$5)=YEAR(C$6), DAYS360(C$5,C$6,TRUE), DAYS360(C$5,DATE(YEAR(C$5),12,31),TRUE)),0)</f>
         <v>29</v>
       </c>
       <c r="D7" s="17">
-        <f t="shared" ref="D7:BI7" si="0">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(D$5,DATE(YEAR(D$5),12,31), TRUE),0)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E7" s="17">
@@ -945,119 +969,119 @@
         <v>359</v>
       </c>
       <c r="AG7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(AND(AG$5 &lt;&gt;"", AG$6 &lt;&gt; ""), IF(YEAR(AG$5)=YEAR(AG$6), DAYS360(AG$5,AG$6,TRUE), DAYS360(AG$5,DATE(YEAR(AG$5),12,31),TRUE)),0)</f>
+        <v>301</v>
       </c>
       <c r="AH7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="AH7:BI7" si="1">IF(AND(AH$5 &lt;&gt;"", AH$6 &lt;&gt; ""), IF(YEAR(AH$5)=YEAR(AH$6), DAYS360(AH$5,AH$6,TRUE), DAYS360(AH$5,DATE(YEAR(AH$5),12,31),TRUE)),0)</f>
+        <v>300</v>
       </c>
       <c r="AI7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="AJ7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
       <c r="AK7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="AL7" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>209</v>
       </c>
       <c r="AM7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AW7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AY7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AZ7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1066,239 +1090,239 @@
         <v>16</v>
       </c>
       <c r="C8" s="16">
-        <f t="shared" ref="C8:AH8" si="1">ROUND(C$7*ZINSSATZ*WERT/360,2)</f>
+        <f t="shared" ref="C8:AH8" si="2">ROUND(C$7*ZINSSATZ*WERT/360,2)</f>
         <v>0.81</v>
       </c>
       <c r="D8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.17</v>
       </c>
       <c r="F8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.17</v>
       </c>
       <c r="I8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.17</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.36</v>
       </c>
       <c r="K8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.67</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.83</v>
       </c>
       <c r="N8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.17</v>
       </c>
       <c r="P8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.33</v>
       </c>
       <c r="Q8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="R8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="S8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83</v>
       </c>
       <c r="T8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AA8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.9700000000000006</v>
       </c>
       <c r="AG8" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8.36</v>
       </c>
       <c r="AH8" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8.33</v>
       </c>
       <c r="AI8" s="16">
-        <f t="shared" ref="AI8:BI8" si="2">ROUND(AI$7*ZINSSATZ*WERT/360,2)</f>
-        <v>0</v>
+        <f t="shared" ref="AI8:BI8" si="3">ROUND(AI$7*ZINSSATZ*WERT/360,2)</f>
+        <v>1.22</v>
       </c>
       <c r="AJ8" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1.28</v>
       </c>
       <c r="AK8" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AL8" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>5.81</v>
       </c>
       <c r="AM8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AN8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AR8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AS8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AT8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AU8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AV8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AW8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AX8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AY8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AZ8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BA8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BB8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BC8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BD8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BE8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BG8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BH8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BI8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1307,239 +1331,239 @@
         <v>12</v>
       </c>
       <c r="C9" s="17">
-        <f>IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),MAX(YEAR(C$6)-YEAR(C$5)-1,0),0)</f>
+        <f t="shared" ref="C9:BM9" si="4">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),MAX(YEAR(C$6)-YEAR(C$5)-1,0),0)</f>
         <v>1</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" ref="D9:BI9" si="3">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),MAX(YEAR(D$6)-YEAR(D$5)-1,0),0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="W9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="X9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="Y9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="Z9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AA9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AB9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AC9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="AD9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="AE9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="AF9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="AG9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AK9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AL9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AO9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AP9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AQ9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AR9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AS9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AT9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AV9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AW9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AX9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AY9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AZ9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BA9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BC9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BD9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BE9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BG9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BI9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1548,239 +1572,239 @@
         <v>17</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" ref="C10:AH10" si="4" xml:space="preserve"> ROUND(-WERT-C$8+(WERT+C$8)*(1+ZINSSATZ)^C$9,2)</f>
+        <f t="shared" ref="C10:AH10" si="5" xml:space="preserve"> ROUND(-WERT-C$8+(WERT+C$8)*(1+ZINSSATZ)^C$9,2)</f>
         <v>10.08</v>
       </c>
       <c r="D10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10.08</v>
       </c>
       <c r="E10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="V10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="X10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.1</v>
       </c>
       <c r="Y10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.1</v>
       </c>
       <c r="Z10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.76</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46.41</v>
       </c>
       <c r="AB10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46.41</v>
       </c>
       <c r="AC10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61.05</v>
       </c>
       <c r="AD10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>114.36</v>
       </c>
       <c r="AE10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>114.36</v>
       </c>
       <c r="AF10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149.33000000000001</v>
       </c>
       <c r="AG10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH10" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AI10" s="12">
-        <f t="shared" ref="AI10:BI10" si="5" xml:space="preserve"> ROUND(-WERT-AI$8+(WERT+AI$8)*(1+ZINSSATZ)^AI$9,2)</f>
+        <f t="shared" ref="AI10:BI10" si="6" xml:space="preserve"> ROUND(-WERT-AI$8+(WERT+AI$8)*(1+ZINSSATZ)^AI$9,2)</f>
         <v>0</v>
       </c>
       <c r="AJ10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AK10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AL10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AM10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AN10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AO10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AQ10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AR10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AS10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AT10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AU10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AV10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AW10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AX10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AY10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AZ10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BA10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BB10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BC10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BD10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BE10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BF10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BG10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BH10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BI10" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1789,239 +1813,239 @@
         <v>18</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" ref="C11:AH11" si="6">ROUND(C$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" ref="C11:AH11" si="7">ROUND(C$9*WERT*ZINSSATZ,2)</f>
         <v>10</v>
       </c>
       <c r="D11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="E11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="H11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="V11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="W11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="X11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="Y11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="Z11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="AA11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="AB11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="AC11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="AD11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="AE11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="AF11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="AG11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH11" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI11" s="12">
-        <f t="shared" ref="AI11:BI11" si="7">ROUND(AI$9*WERT*ZINSSATZ,2)</f>
+        <f t="shared" ref="AI11:BI11" si="8">ROUND(AI$9*WERT*ZINSSATZ,2)</f>
         <v>0</v>
       </c>
       <c r="AJ11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AK11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AL11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AM11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AN11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AP11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AQ11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AS11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AT11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AU11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AV11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AY11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AZ11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BA11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BC11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BD11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BE11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BF11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BG11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BH11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BI11" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -2034,235 +2058,235 @@
         <v>30</v>
       </c>
       <c r="D12" s="17">
-        <f t="shared" ref="D12:BI12" si="8">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
+        <f t="shared" ref="D12:BI12" si="9">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="E12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>61</v>
       </c>
       <c r="F12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="G12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="H12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>58</v>
       </c>
       <c r="I12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="J12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>61</v>
       </c>
       <c r="K12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
       <c r="L12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>121</v>
       </c>
       <c r="M12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>151</v>
       </c>
       <c r="N12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>181</v>
       </c>
       <c r="O12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>211</v>
       </c>
       <c r="P12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>241</v>
       </c>
       <c r="Q12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>271</v>
       </c>
       <c r="R12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>301</v>
       </c>
       <c r="S12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>331</v>
       </c>
       <c r="T12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="U12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="V12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="W12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="X12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Y12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="Z12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="AA12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AB12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="AC12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AD12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>58</v>
       </c>
       <c r="AE12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="AF12" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(AND(AF$5 &lt;&gt;"", AF$6 &lt;&gt; ""),IF(YEAR(AF$5)=YEAR(AF$6),0, DAYS360(DATE(YEAR(AF$6),1,1)-1,AF$6, TRUE)),0)</f>
         <v>1</v>
       </c>
       <c r="AG12" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(AND(AG$5 &lt;&gt;"", AG$6 &lt;&gt; ""),IF(YEAR(AG$5)=YEAR(AG$6),0, DAYS360(DATE(YEAR(AG$6),1,1)-1,AG$6, TRUE)),0)</f>
         <v>0</v>
       </c>
       <c r="AH12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AH12:BI12" si="10">IF(AND(AH$5 &lt;&gt;"", AH$6 &lt;&gt; ""),IF(YEAR(AH$5)=YEAR(AH$6),0, DAYS360(DATE(YEAR(AH$6),1,1)-1,AH$6, TRUE)),0)</f>
         <v>0</v>
       </c>
       <c r="AI12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AM12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AN12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AO12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AP12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AQ12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AR12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AS12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AT12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AU12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AV12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AW12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AX12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AY12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AZ12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BA12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BB12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BC12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BD12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BE12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BF12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BG12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BH12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BI12" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -2271,239 +2295,239 @@
         <v>19</v>
       </c>
       <c r="C13" s="16">
-        <f t="shared" ref="C13:AH13" si="9">ROUND((WERT+C$8+C$10)*C$12/360*ZINSSATZ,2)</f>
+        <f t="shared" ref="C13:AH13" si="11">ROUND((WERT+C$8+C$10)*C$12/360*ZINSSATZ,2)</f>
         <v>0.92</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.85</v>
       </c>
       <c r="F13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="G13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.92</v>
       </c>
       <c r="H13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.76</v>
       </c>
       <c r="I13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.94</v>
       </c>
       <c r="J13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.84</v>
       </c>
       <c r="K13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.72</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.59</v>
       </c>
       <c r="M13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.4400000000000004</v>
       </c>
       <c r="N13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.28</v>
       </c>
       <c r="O13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.11</v>
       </c>
       <c r="P13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.92</v>
       </c>
       <c r="Q13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.72</v>
       </c>
       <c r="R13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>8.5</v>
       </c>
       <c r="S13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.27</v>
       </c>
       <c r="T13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="U13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.5</v>
       </c>
       <c r="V13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.03</v>
       </c>
       <c r="W13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.05</v>
       </c>
       <c r="X13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.04</v>
       </c>
       <c r="Y13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.66</v>
       </c>
       <c r="Z13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>13.98</v>
       </c>
       <c r="AA13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.04</v>
       </c>
       <c r="AB13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.32</v>
       </c>
       <c r="AC13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.04</v>
       </c>
       <c r="AD13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.45</v>
       </c>
       <c r="AE13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.51</v>
       </c>
       <c r="AF13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AG13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AH13" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AI13" s="16">
-        <f t="shared" ref="AI13:BI13" si="10">ROUND((WERT+AI$8+AI$10)*AI$12/360*ZINSSATZ,2)</f>
+        <f t="shared" ref="AI13:BI13" si="12">ROUND((WERT+AI$8+AI$10)*AI$12/360*ZINSSATZ,2)</f>
         <v>0</v>
       </c>
       <c r="AJ13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AL13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AM13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AN13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AO13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AP13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AQ13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AR13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AS13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AT13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AU13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AV13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AW13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AX13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AY13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AZ13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BA13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BC13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BD13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BE13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BF13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BG13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BH13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BI13" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -2512,239 +2536,239 @@
         <v>20</v>
       </c>
       <c r="C14" s="16">
-        <f t="shared" ref="C14:AH14" si="11">ROUND(WERT*ZINSSATZ*C$12/360,2)</f>
+        <f t="shared" ref="C14:AH14" si="13">ROUND(WERT*ZINSSATZ*C$12/360,2)</f>
         <v>0.83</v>
       </c>
       <c r="D14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.69</v>
       </c>
       <c r="F14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="G14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.83</v>
       </c>
       <c r="H14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.61</v>
       </c>
       <c r="I14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.86</v>
       </c>
       <c r="J14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.69</v>
       </c>
       <c r="K14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.5299999999999998</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.36</v>
       </c>
       <c r="M14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.1900000000000004</v>
       </c>
       <c r="N14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.03</v>
       </c>
       <c r="O14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.86</v>
       </c>
       <c r="P14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.69</v>
       </c>
       <c r="Q14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.53</v>
       </c>
       <c r="R14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.36</v>
       </c>
       <c r="S14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.19</v>
       </c>
       <c r="T14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="U14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="V14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="W14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="X14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="Y14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="Z14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="AA14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="AB14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="AC14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="AD14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.61</v>
       </c>
       <c r="AE14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.64</v>
       </c>
       <c r="AF14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.03</v>
       </c>
       <c r="AG14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AH14" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI14" s="16">
-        <f t="shared" ref="AI14:BI14" si="12">ROUND(WERT*ZINSSATZ*AI$12/360,2)</f>
+        <f t="shared" ref="AI14:BI14" si="14">ROUND(WERT*ZINSSATZ*AI$12/360,2)</f>
         <v>0</v>
       </c>
       <c r="AJ14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AK14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AL14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AN14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AO14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AP14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AQ14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AR14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AS14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AT14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AU14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AV14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AW14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AX14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AY14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AZ14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BA14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BB14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BC14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BD14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BE14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BF14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BG14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BH14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BI14" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -2760,235 +2784,235 @@
         <v>11.81</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" ref="D15:BI15" si="13">ROUND(D$8+D$10+D$13,2)</f>
+        <f t="shared" ref="D15:BI15" si="15">ROUND(D$8+D$10+D$13,2)</f>
         <v>10.92</v>
       </c>
       <c r="E15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>11.02</v>
       </c>
       <c r="F15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.92</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.93</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.11</v>
       </c>
       <c r="J15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.199999999999999</v>
       </c>
       <c r="K15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.220000000000001</v>
       </c>
       <c r="L15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.26</v>
       </c>
       <c r="M15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.27</v>
       </c>
       <c r="N15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.28</v>
       </c>
       <c r="O15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.28</v>
       </c>
       <c r="P15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.25</v>
       </c>
       <c r="Q15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.220000000000001</v>
       </c>
       <c r="R15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.17</v>
       </c>
       <c r="S15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10.1</v>
       </c>
       <c r="T15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="U15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>15.5</v>
       </c>
       <c r="V15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>21.03</v>
       </c>
       <c r="W15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>27.05</v>
       </c>
       <c r="X15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>33.14</v>
       </c>
       <c r="Y15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>39.76</v>
       </c>
       <c r="Z15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>53.74</v>
       </c>
       <c r="AA15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>46.45</v>
       </c>
       <c r="AB15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>53.73</v>
       </c>
       <c r="AC15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>61.09</v>
       </c>
       <c r="AD15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>117.81</v>
       </c>
       <c r="AE15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>117.87</v>
       </c>
       <c r="AF15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>159.37</v>
       </c>
       <c r="AG15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>8.36</v>
       </c>
       <c r="AH15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>8.33</v>
       </c>
       <c r="AI15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>1.22</v>
       </c>
       <c r="AJ15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>1.28</v>
       </c>
       <c r="AK15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AL15" s="19">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>5.81</v>
       </c>
       <c r="AM15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AO15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AP15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AQ15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AR15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AS15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AT15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AU15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AV15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AW15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AX15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AY15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AZ15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BA15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BB15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BC15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BD15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BE15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BF15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BG15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BH15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BI15" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3001,235 +3025,361 @@
         <v>11.64</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" ref="D16:BI16" si="14">ROUND(D$8+D$11+D$14,2)</f>
+        <f t="shared" ref="D16:BI16" si="16">ROUND(D$8+D$11+D$14,2)</f>
         <v>10.84</v>
       </c>
       <c r="E16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.86</v>
       </c>
       <c r="F16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="G16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.83</v>
       </c>
       <c r="H16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.78</v>
       </c>
       <c r="I16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="J16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.050000000000001</v>
       </c>
       <c r="K16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="L16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="M16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.02</v>
       </c>
       <c r="N16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="O16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="P16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.02</v>
       </c>
       <c r="Q16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="R16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.029999999999999</v>
       </c>
       <c r="S16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.02</v>
       </c>
       <c r="T16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="U16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>15</v>
       </c>
       <c r="V16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>20.03</v>
       </c>
       <c r="W16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>25</v>
       </c>
       <c r="X16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30.03</v>
       </c>
       <c r="Y16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>35</v>
       </c>
       <c r="Z16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="AA16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>40.03</v>
       </c>
       <c r="AB16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="AC16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>50.03</v>
       </c>
       <c r="AD16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>81.61</v>
       </c>
       <c r="AE16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>81.64</v>
       </c>
       <c r="AF16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="AG16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>8.36</v>
       </c>
       <c r="AH16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>8.33</v>
       </c>
       <c r="AI16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1.22</v>
       </c>
       <c r="AJ16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1.28</v>
       </c>
       <c r="AK16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AL16" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>5.81</v>
       </c>
       <c r="AM16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AO16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AP16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AQ16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AR16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AS16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AT16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AU16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AV16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AW16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AX16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AY16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AZ16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BA16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BB16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BC16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BD16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BE16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BF16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BG16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BH16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="BI16" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="C19" s="12">
+        <f t="shared" ref="C19:AF19" si="17">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),IF(YEAR(C$5)=YEAR(C$6),0, DAYS360(DATE(YEAR(C$6),1,1)-1,C$6, TRUE)),0)</f>
+        <v>30</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="17"/>
+        <v>61</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="17"/>
+        <v>360</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="17"/>
+        <v>58</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="17"/>
+        <v>31</v>
+      </c>
+      <c r="J19" s="12">
+        <f t="shared" si="17"/>
+        <v>61</v>
+      </c>
+      <c r="K19" s="12">
+        <f t="shared" si="17"/>
+        <v>91</v>
+      </c>
+      <c r="L19" s="12">
+        <f t="shared" si="17"/>
+        <v>121</v>
+      </c>
+      <c r="M19" s="12">
+        <f t="shared" si="17"/>
+        <v>151</v>
+      </c>
+      <c r="N19" s="12">
+        <f t="shared" si="17"/>
+        <v>181</v>
+      </c>
+      <c r="O19" s="12">
+        <f t="shared" si="17"/>
+        <v>211</v>
+      </c>
+      <c r="P19" s="12">
+        <f t="shared" si="17"/>
+        <v>241</v>
+      </c>
+      <c r="Q19" s="12">
+        <f t="shared" si="17"/>
+        <v>271</v>
+      </c>
+      <c r="R19" s="12">
+        <f t="shared" si="17"/>
+        <v>301</v>
+      </c>
+      <c r="S19" s="12">
+        <f t="shared" si="17"/>
+        <v>331</v>
+      </c>
+      <c r="T19" s="12">
+        <f t="shared" si="17"/>
+        <v>180</v>
+      </c>
+      <c r="U19" s="12">
+        <f t="shared" si="17"/>
+        <v>180</v>
+      </c>
+      <c r="V19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="W19" s="12">
+        <f t="shared" si="17"/>
+        <v>180</v>
+      </c>
+      <c r="X19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="Y19" s="12">
+        <f t="shared" si="17"/>
+        <v>180</v>
+      </c>
+      <c r="Z19" s="12">
+        <f t="shared" si="17"/>
+        <v>360</v>
+      </c>
+      <c r="AA19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="AB19" s="12">
+        <f t="shared" si="17"/>
+        <v>180</v>
+      </c>
+      <c r="AC19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="AD19" s="12">
+        <f t="shared" si="17"/>
+        <v>58</v>
+      </c>
+      <c r="AE19" s="12">
+        <f t="shared" si="17"/>
+        <v>59</v>
+      </c>
+      <c r="AF19" s="12">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <f>IF(AND(AG$5 &lt;&gt;"", AG$6 &lt;&gt; ""),IF(YEAR(AG$5)=YEAR(AG$6),0, DAYS360(DATE(YEAR(AG$6),1,1)-1,AG$6, TRUE)),0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more tests, correct feb intrest calculation
</commit_message>
<xml_diff>
--- a/DOCS/ZinsBerechnung.xlsx
+++ b/DOCS/ZinsBerechnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\qt-dev\home\dev\DKV2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0A702E37-44F8-47D0-A9BA-6D58917473C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2B78E8FB-A198-4380-80E7-39A505FE0C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="765" windowWidth="18810" windowHeight="14055" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
+    <workbookView xWindow="9885" yWindow="1380" windowWidth="18810" windowHeight="14055" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zinseszins" sheetId="3" r:id="rId1"/>
@@ -539,10 +539,10 @@
   <dimension ref="A2:BI19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AG5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AJ5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AL7" sqref="AL7"/>
+      <selection pane="bottomRight" activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="38" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:61" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -683,11 +683,21 @@
       <c r="AL5" s="15" t="d">
         <v>2014-06-01</v>
       </c>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="14"/>
+      <c r="AM5" s="15" t="d">
+        <v>2016-02-28</v>
+      </c>
+      <c r="AN5" s="15" t="d">
+        <v>2016-02-29</v>
+      </c>
+      <c r="AO5" s="15" t="d">
+        <v>2016-03-01</v>
+      </c>
+      <c r="AP5" s="15" t="d">
+        <v>2015-02-28</v>
+      </c>
+      <c r="AQ5" s="15" t="d">
+        <v>2015-03-01</v>
+      </c>
       <c r="AR5" s="14"/>
       <c r="AS5" s="14"/>
       <c r="AT5" s="14"/>
@@ -820,11 +830,21 @@
       <c r="AL6" s="15" t="d">
         <v>2014-12-31</v>
       </c>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="14"/>
+      <c r="AM6" s="15" t="d">
+        <v>2016-03-30</v>
+      </c>
+      <c r="AN6" s="15" t="d">
+        <v>2016-03-30</v>
+      </c>
+      <c r="AO6" s="15" t="d">
+        <v>2016-03-30</v>
+      </c>
+      <c r="AP6" s="15" t="d">
+        <v>2015-03-30</v>
+      </c>
+      <c r="AQ6" s="15" t="d">
+        <v>2015-03-30</v>
+      </c>
       <c r="AR6" s="14"/>
       <c r="AS6" s="14"/>
       <c r="AT6" s="14"/>
@@ -994,23 +1014,23 @@
       </c>
       <c r="AM7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AN7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AO7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AP7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AQ7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AR7" s="17">
         <f t="shared" si="1"/>
@@ -1235,23 +1255,23 @@
       </c>
       <c r="AM8" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AN8" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="AO8" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AP8" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AQ8" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AR8" s="16">
         <f t="shared" si="3"/>
@@ -1331,7 +1351,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="17">
-        <f t="shared" ref="C9:BM9" si="4">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),MAX(YEAR(C$6)-YEAR(C$5)-1,0),0)</f>
+        <f t="shared" ref="C9:BI9" si="4">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),MAX(YEAR(C$6)-YEAR(C$5)-1,0),0)</f>
         <v>1</v>
       </c>
       <c r="D9" s="17">
@@ -2058,7 +2078,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="17">
-        <f t="shared" ref="D12:BI12" si="9">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
+        <f t="shared" ref="D12:AE12" si="9">IF(AND(D$5 &lt;&gt;"", D$6 &lt;&gt; ""),DAYS360(DATE(YEAR(D$6),1,1)-1,D$6, FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="E12" s="17">
@@ -2925,23 +2945,23 @@
       </c>
       <c r="AM15" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AN15" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="AO15" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AP15" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AQ15" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AR15" s="19">
         <f t="shared" si="15"/>
@@ -3166,23 +3186,23 @@
       </c>
       <c r="AM16" s="19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AN16" s="19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="AO16" s="19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AP16" s="19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="AQ16" s="19">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="AR16" s="19">
         <f t="shared" si="16"/>

</xml_diff>

<commit_message>
finish contract activities remove rounding error from interest calculation
</commit_message>
<xml_diff>
--- a/DOCS/ZinsBerechnung.xlsx
+++ b/DOCS/ZinsBerechnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\qt-dev\home\dev\DKV2\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Qt-dev\home\dev\DKV2.c_h\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2B78E8FB-A198-4380-80E7-39A505FE0C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{95C9EDC5-308C-436E-AFE1-F13C20F4972C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="1380" windowWidth="18810" windowHeight="14055" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
+    <workbookView xWindow="-156" yWindow="1068" windowWidth="13260" windowHeight="12660" xr2:uid="{DAE5B99E-0AB9-4583-8B56-1821172FA1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zinseszins" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -111,8 +113,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -189,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -222,6 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,23 +543,23 @@
   <dimension ref="A2:BI19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AJ5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AN7" sqref="AN7"/>
+      <selection pane="bottomRight" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="43" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:61" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
@@ -563,7 +567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
@@ -571,7 +575,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
@@ -717,7 +721,7 @@
       <c r="BH5" s="14"/>
       <c r="BI5" s="14"/>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>10</v>
       </c>
@@ -864,7 +868,7 @@
       <c r="BH6" s="14"/>
       <c r="BI6" s="14"/>
     </row>
-    <row r="7" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1114,8 +1118,8 @@
         <v>0.81</v>
       </c>
       <c r="D8" s="16">
-        <f t="shared" si="2"/>
-        <v>0.81</v>
+        <f>D$7*ZINSSATZ*WERT/360</f>
+        <v>0.80555555555555569</v>
       </c>
       <c r="E8" s="16">
         <f t="shared" si="2"/>
@@ -1138,32 +1142,32 @@
         <v>9.17</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" si="2"/>
-        <v>8.36</v>
+        <f>J$7*ZINSSATZ*WERT/360</f>
+        <v>8.3611111111111107</v>
       </c>
       <c r="K8" s="16">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="L8" s="16">
-        <f t="shared" si="2"/>
-        <v>6.67</v>
+      <c r="L8" s="20">
+        <f>L$7*ZINSSATZ*WERT/360</f>
+        <v>6.666666666666667</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" si="2"/>
-        <v>5.83</v>
+        <f>M$7*ZINSSATZ*WERT/360</f>
+        <v>5.833333333333333</v>
       </c>
       <c r="N8" s="16">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O8" s="16">
-        <f t="shared" si="2"/>
-        <v>4.17</v>
+        <f>O$7*ZINSSATZ*WERT/360</f>
+        <v>4.166666666666667</v>
       </c>
       <c r="P8" s="16">
-        <f t="shared" si="2"/>
-        <v>3.33</v>
+        <f>P$7*ZINSSATZ*WERT/360</f>
+        <v>3.3333333333333335</v>
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="2"/>
@@ -1174,8 +1178,8 @@
         <v>1.67</v>
       </c>
       <c r="S8" s="16">
-        <f t="shared" si="2"/>
-        <v>0.83</v>
+        <f>S$7*ZINSSATZ*WERT/360</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="T8" s="16">
         <f t="shared" si="2"/>
@@ -1202,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="Z8" s="16">
-        <f t="shared" si="2"/>
+        <f>Z$7*ZINSSATZ*WERT/360</f>
         <v>5</v>
       </c>
       <c r="AA8" s="16">
@@ -1226,8 +1230,8 @@
         <v>0</v>
       </c>
       <c r="AF8" s="16">
-        <f t="shared" si="2"/>
-        <v>9.9700000000000006</v>
+        <f>AF$7*ZINSSATZ*WERT/360</f>
+        <v>9.9722222222222214</v>
       </c>
       <c r="AG8" s="16">
         <f t="shared" si="2"/>
@@ -1346,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
@@ -1587,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>17</v>
       </c>
@@ -1596,8 +1600,8 @@
         <v>10.08</v>
       </c>
       <c r="D10" s="12">
-        <f t="shared" si="5"/>
-        <v>10.08</v>
+        <f xml:space="preserve"> -WERT-D$8+(WERT+D$8)*(1+ZINSSATZ)^D$9</f>
+        <v>10.080555555555563</v>
       </c>
       <c r="E10" s="12">
         <f t="shared" si="5"/>
@@ -1684,8 +1688,8 @@
         <v>33.1</v>
       </c>
       <c r="Z10" s="12">
-        <f t="shared" si="5"/>
-        <v>34.76</v>
+        <f xml:space="preserve"> -WERT-Z$8+(WERT+Z$8)*(1+ZINSSATZ)^Z$9</f>
+        <v>34.755000000000052</v>
       </c>
       <c r="AA10" s="12">
         <f t="shared" si="5"/>
@@ -1696,8 +1700,8 @@
         <v>46.41</v>
       </c>
       <c r="AC10" s="12">
-        <f t="shared" si="5"/>
-        <v>61.05</v>
+        <f xml:space="preserve"> -WERT-AC$8+(WERT+AC$8)*(1+ZINSSATZ)^AC$9</f>
+        <v>61.051000000000045</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="5"/>
@@ -1708,8 +1712,8 @@
         <v>114.36</v>
       </c>
       <c r="AF10" s="12">
-        <f t="shared" si="5"/>
-        <v>149.33000000000001</v>
+        <f xml:space="preserve"> -WERT-AF$8+(WERT+AF$8)*(1+ZINSSATZ)^AF$9</f>
+        <v>149.33652524080571</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="5"/>
@@ -1828,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="Z11" s="12">
-        <f t="shared" si="7"/>
+        <f>Z$9*WERT*ZINSSATZ</f>
         <v>30</v>
       </c>
       <c r="AA11" s="12">
@@ -1949,7 +1953,7 @@
         <v>80</v>
       </c>
       <c r="AF11" s="12">
-        <f t="shared" si="7"/>
+        <f>AF$9*WERT*ZINSSATZ</f>
         <v>90</v>
       </c>
       <c r="AG11" s="12">
@@ -2069,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>13</v>
       </c>
@@ -2310,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
@@ -2319,8 +2323,8 @@
         <v>0.92</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" si="11"/>
-        <v>0.03</v>
+        <f>(WERT+D$8+D$10)*D$12/360*ZINSSATZ</f>
+        <v>3.0801697530864203E-2</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="11"/>
@@ -2343,32 +2347,32 @@
         <v>0.94</v>
       </c>
       <c r="J13" s="16">
-        <f t="shared" si="11"/>
-        <v>1.84</v>
+        <f>(WERT+J$8+J$10)*J$12/360*ZINSSATZ</f>
+        <v>1.8361188271604938</v>
       </c>
       <c r="K13" s="16">
         <f t="shared" si="11"/>
         <v>2.72</v>
       </c>
-      <c r="L13" s="16">
-        <f t="shared" si="11"/>
-        <v>3.59</v>
+      <c r="L13" s="20">
+        <f>(WERT+L$8+L$10)*L$12/360*ZINSSATZ</f>
+        <v>3.5851851851851855</v>
       </c>
       <c r="M13" s="16">
-        <f t="shared" si="11"/>
-        <v>4.4400000000000004</v>
+        <f>(WERT+M$8+M$10)*M$12/360*ZINSSATZ</f>
+        <v>4.4391203703703708</v>
       </c>
       <c r="N13" s="16">
         <f t="shared" si="11"/>
         <v>5.28</v>
       </c>
       <c r="O13" s="16">
-        <f t="shared" si="11"/>
-        <v>6.11</v>
+        <f>(WERT+O$8+O$10)*O$12/360*ZINSSATZ</f>
+        <v>6.1053240740740753</v>
       </c>
       <c r="P13" s="16">
-        <f t="shared" si="11"/>
-        <v>6.92</v>
+        <f>(WERT+P$8+P$10)*P$12/360*ZINSSATZ</f>
+        <v>6.9175925925925927</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" si="11"/>
@@ -2379,8 +2383,8 @@
         <v>8.5</v>
       </c>
       <c r="S13" s="16">
-        <f t="shared" si="11"/>
-        <v>9.27</v>
+        <f>(WERT+S$8+S$10)*S$12/360*ZINSSATZ</f>
+        <v>9.2710648148148138</v>
       </c>
       <c r="T13" s="16">
         <f t="shared" si="11"/>
@@ -2407,8 +2411,8 @@
         <v>6.66</v>
       </c>
       <c r="Z13" s="16">
-        <f t="shared" si="11"/>
-        <v>13.98</v>
+        <f>(WERT+Z$8+Z$10)*Z$12/360*ZINSSATZ</f>
+        <v>13.975500000000006</v>
       </c>
       <c r="AA13" s="16">
         <f t="shared" si="11"/>
@@ -2419,8 +2423,8 @@
         <v>7.32</v>
       </c>
       <c r="AC13" s="16">
-        <f t="shared" si="11"/>
-        <v>0.04</v>
+        <f>(WERT+AC$8+AC$10)*AC$12/360*ZINSSATZ</f>
+        <v>4.4736388888888902E-2</v>
       </c>
       <c r="AD13" s="16">
         <f t="shared" si="11"/>
@@ -2431,8 +2435,8 @@
         <v>3.51</v>
       </c>
       <c r="AF13" s="16">
-        <f t="shared" si="11"/>
-        <v>7.0000000000000007E-2</v>
+        <f>(WERT+AF$8+AF$10)*AF$12/360*ZINSSATZ</f>
+        <v>7.2030207628618878E-2</v>
       </c>
       <c r="AG13" s="16">
         <f t="shared" si="11"/>
@@ -2551,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>20</v>
       </c>
@@ -2560,8 +2564,8 @@
         <v>0.83</v>
       </c>
       <c r="D14" s="16">
-        <f t="shared" si="13"/>
-        <v>0.03</v>
+        <f>WERT*ZINSSATZ*D$12/360</f>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" si="13"/>
@@ -2584,32 +2588,32 @@
         <v>0.86</v>
       </c>
       <c r="J14" s="16">
-        <f t="shared" si="13"/>
-        <v>1.69</v>
+        <f>WERT*ZINSSATZ*J$12/360</f>
+        <v>1.6944444444444444</v>
       </c>
       <c r="K14" s="16">
         <f t="shared" si="13"/>
         <v>2.5299999999999998</v>
       </c>
-      <c r="L14" s="16">
-        <f t="shared" si="13"/>
-        <v>3.36</v>
+      <c r="L14" s="20">
+        <f>WERT*ZINSSATZ*L$12/360</f>
+        <v>3.3611111111111112</v>
       </c>
       <c r="M14" s="16">
-        <f t="shared" si="13"/>
-        <v>4.1900000000000004</v>
+        <f>WERT*ZINSSATZ*M$12/360</f>
+        <v>4.1944444444444446</v>
       </c>
       <c r="N14" s="16">
         <f t="shared" si="13"/>
         <v>5.03</v>
       </c>
       <c r="O14" s="16">
-        <f t="shared" si="13"/>
-        <v>5.86</v>
+        <f>WERT*ZINSSATZ*O$12/360</f>
+        <v>5.8611111111111107</v>
       </c>
       <c r="P14" s="16">
-        <f t="shared" si="13"/>
-        <v>6.69</v>
+        <f>WERT*ZINSSATZ*P$12/360</f>
+        <v>6.6944444444444446</v>
       </c>
       <c r="Q14" s="16">
         <f t="shared" si="13"/>
@@ -2620,8 +2624,8 @@
         <v>8.36</v>
       </c>
       <c r="S14" s="16">
-        <f t="shared" si="13"/>
-        <v>9.19</v>
+        <f>WERT*ZINSSATZ*S$12/360</f>
+        <v>9.1944444444444446</v>
       </c>
       <c r="T14" s="16">
         <f t="shared" si="13"/>
@@ -2648,7 +2652,7 @@
         <v>5</v>
       </c>
       <c r="Z14" s="16">
-        <f t="shared" si="13"/>
+        <f>WERT*ZINSSATZ*Z$12/360</f>
         <v>10</v>
       </c>
       <c r="AA14" s="16">
@@ -2660,8 +2664,8 @@
         <v>5</v>
       </c>
       <c r="AC14" s="16">
-        <f t="shared" si="13"/>
-        <v>0.03</v>
+        <f>WERT*ZINSSATZ*AC$12/360</f>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="AD14" s="16">
         <f t="shared" si="13"/>
@@ -2672,8 +2676,8 @@
         <v>1.64</v>
       </c>
       <c r="AF14" s="16">
-        <f t="shared" si="13"/>
-        <v>0.03</v>
+        <f>WERT*ZINSSATZ*AF$12/360</f>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="AG14" s="16">
         <f t="shared" si="13"/>
@@ -2792,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2837,7 +2841,7 @@
       </c>
       <c r="L15" s="19">
         <f t="shared" si="15"/>
-        <v>10.26</v>
+        <v>10.25</v>
       </c>
       <c r="M15" s="19">
         <f t="shared" si="15"/>
@@ -2849,7 +2853,7 @@
       </c>
       <c r="O15" s="19">
         <f t="shared" si="15"/>
-        <v>10.28</v>
+        <v>10.27</v>
       </c>
       <c r="P15" s="19">
         <f t="shared" si="15"/>
@@ -2893,7 +2897,7 @@
       </c>
       <c r="Z15" s="19">
         <f t="shared" si="15"/>
-        <v>53.74</v>
+        <v>53.73</v>
       </c>
       <c r="AA15" s="19">
         <f t="shared" si="15"/>
@@ -2905,7 +2909,7 @@
       </c>
       <c r="AC15" s="19">
         <f t="shared" si="15"/>
-        <v>61.09</v>
+        <v>61.1</v>
       </c>
       <c r="AD15" s="19">
         <f t="shared" si="15"/>
@@ -2917,7 +2921,7 @@
       </c>
       <c r="AF15" s="19">
         <f t="shared" si="15"/>
-        <v>159.37</v>
+        <v>159.38</v>
       </c>
       <c r="AG15" s="19">
         <f t="shared" si="15"/>
@@ -3036,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
@@ -3046,7 +3050,7 @@
       </c>
       <c r="D16" s="19">
         <f t="shared" ref="D16:BI16" si="16">ROUND(D$8+D$11+D$14,2)</f>
-        <v>10.84</v>
+        <v>10.83</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="16"/>
@@ -3070,7 +3074,7 @@
       </c>
       <c r="J16" s="19">
         <f t="shared" si="16"/>
-        <v>10.050000000000001</v>
+        <v>10.06</v>
       </c>
       <c r="K16" s="19">
         <f t="shared" si="16"/>
@@ -3082,7 +3086,7 @@
       </c>
       <c r="M16" s="19">
         <f t="shared" si="16"/>
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="N16" s="19">
         <f t="shared" si="16"/>
@@ -3094,7 +3098,7 @@
       </c>
       <c r="P16" s="19">
         <f t="shared" si="16"/>
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="Q16" s="19">
         <f t="shared" si="16"/>
@@ -3106,7 +3110,7 @@
       </c>
       <c r="S16" s="19">
         <f t="shared" si="16"/>
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="T16" s="19">
         <f t="shared" si="16"/>
@@ -3277,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:33" x14ac:dyDescent="0.3">
       <c r="C19" s="12">
         <f t="shared" ref="C19:AF19" si="17">IF(AND(C$5 &lt;&gt;"", C$6 &lt;&gt; ""),IF(YEAR(C$5)=YEAR(C$6),0, DAYS360(DATE(YEAR(C$6),1,1)-1,C$6, TRUE)),0)</f>
         <v>30</v>
@@ -3417,24 +3421,24 @@
       <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.109375" customWidth="1"/>
+    <col min="21" max="21" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3476,7 +3480,7 @@
         <v>2017-12-31</v>
       </c>
     </row>
-    <row r="3" spans="4:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:22" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3490,7 +3494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:22" x14ac:dyDescent="0.3">
       <c r="F4" s="6" t="s">
         <v>1</v>
       </c>
@@ -3521,7 +3525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:22" x14ac:dyDescent="0.3">
       <c r="F5" s="8" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3557,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="d">
         <f>DATE(E2,1,1)</f>
         <v>2016-01-01</v>
@@ -3605,7 +3609,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E7" s="1" t="d">
         <f>E6+1</f>
         <v>2016-01-02</v>
@@ -3653,7 +3657,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="d">
         <f t="shared" ref="E8:E71" si="5">E7+1</f>
         <v>2016-01-03</v>
@@ -3701,7 +3705,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E9" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-04</v>
@@ -3746,7 +3750,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-05</v>
@@ -3788,7 +3792,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-06</v>
@@ -3830,7 +3834,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-07</v>
@@ -3872,7 +3876,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-08</v>
@@ -3914,7 +3918,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-09</v>
@@ -3956,7 +3960,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E15" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-10</v>
@@ -3998,7 +4002,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:22" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-11</v>
@@ -4040,7 +4044,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E17" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-12</v>
@@ -4082,7 +4086,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E18" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-13</v>
@@ -4124,7 +4128,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E19" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-14</v>
@@ -4166,7 +4170,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E20" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-15</v>
@@ -4208,7 +4212,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E21" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-16</v>
@@ -4250,7 +4254,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-17</v>
@@ -4292,7 +4296,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E23" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-18</v>
@@ -4334,7 +4338,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E24" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-19</v>
@@ -4376,7 +4380,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E25" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-20</v>
@@ -4418,7 +4422,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-21</v>
@@ -4460,7 +4464,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E27" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-22</v>
@@ -4502,7 +4506,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-23</v>
@@ -4544,7 +4548,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E29" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-24</v>
@@ -4586,7 +4590,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E30" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-25</v>
@@ -4628,7 +4632,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-26</v>
@@ -4670,7 +4674,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E32" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-27</v>
@@ -4712,7 +4716,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E33" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-28</v>
@@ -4754,7 +4758,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="34" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E34" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-29</v>
@@ -4796,7 +4800,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E35" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-30</v>
@@ -4841,7 +4845,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="36" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E36" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-01-31</v>
@@ -4886,7 +4890,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E37" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-01</v>
@@ -4934,7 +4938,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="38" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E38" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-02</v>
@@ -4982,7 +4986,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="39" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-03</v>
@@ -5024,7 +5028,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="40" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E40" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-04</v>
@@ -5066,7 +5070,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="41" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E41" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-05</v>
@@ -5108,7 +5112,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E42" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-06</v>
@@ -5150,7 +5154,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="43" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E43" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-07</v>
@@ -5192,7 +5196,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="44" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-08</v>
@@ -5234,7 +5238,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="45" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-09</v>
@@ -5276,7 +5280,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E46" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-10</v>
@@ -5318,7 +5322,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="47" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E47" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-11</v>
@@ -5360,7 +5364,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E48" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-12</v>
@@ -5402,7 +5406,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="49" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E49" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-13</v>
@@ -5444,7 +5448,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="50" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-14</v>
@@ -5486,7 +5490,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="51" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E51" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-15</v>
@@ -5528,7 +5532,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E52" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-16</v>
@@ -5570,7 +5574,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="53" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E53" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-17</v>
@@ -5612,7 +5616,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E54" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-18</v>
@@ -5654,7 +5658,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="55" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E55" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-19</v>
@@ -5696,7 +5700,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E56" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-20</v>
@@ -5738,7 +5742,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="57" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E57" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-21</v>
@@ -5780,7 +5784,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="58" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E58" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-22</v>
@@ -5822,7 +5826,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="59" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E59" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-23</v>
@@ -5864,7 +5868,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="60" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E60" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-24</v>
@@ -5906,7 +5910,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="61" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E61" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-25</v>
@@ -5948,7 +5952,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="62" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E62" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-26</v>
@@ -5990,7 +5994,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="63" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-27</v>
@@ -6032,7 +6036,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="64" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E64" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-28</v>
@@ -6077,7 +6081,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E65" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-02-29</v>
@@ -6122,7 +6126,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="66" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E66" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-01</v>
@@ -6167,7 +6171,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E67" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-02</v>
@@ -6212,7 +6216,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E68" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-03</v>
@@ -6254,7 +6258,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="69" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E69" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-04</v>
@@ -6296,7 +6300,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="70" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E70" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-05</v>
@@ -6338,7 +6342,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E71" s="1" t="d">
         <f t="shared" si="5"/>
         <v>2016-03-06</v>
@@ -6380,7 +6384,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E72" s="1" t="d">
         <f t="shared" ref="E72:E135" si="15">E71+1</f>
         <v>2016-03-07</v>
@@ -6422,7 +6426,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="73" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E73" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-08</v>
@@ -6464,7 +6468,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="74" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E74" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-09</v>
@@ -6506,7 +6510,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="75" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E75" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-10</v>
@@ -6548,7 +6552,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="76" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E76" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-11</v>
@@ -6590,7 +6594,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E77" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-12</v>
@@ -6632,7 +6636,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="78" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E78" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-13</v>
@@ -6674,7 +6678,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="79" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E79" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-14</v>
@@ -6716,7 +6720,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="80" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E80" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-15</v>
@@ -6758,7 +6762,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E81" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-16</v>
@@ -6800,7 +6804,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="82" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E82" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-17</v>
@@ -6842,7 +6846,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="83" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E83" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-18</v>
@@ -6884,7 +6888,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E84" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-19</v>
@@ -6926,7 +6930,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E85" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-20</v>
@@ -6968,7 +6972,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E86" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-21</v>
@@ -7010,7 +7014,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="87" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E87" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-22</v>
@@ -7052,7 +7056,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="88" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E88" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-23</v>
@@ -7094,7 +7098,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E89" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-24</v>
@@ -7136,7 +7140,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="90" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E90" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-25</v>
@@ -7178,7 +7182,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E91" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-26</v>
@@ -7220,7 +7224,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="92" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E92" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-27</v>
@@ -7262,7 +7266,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E93" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-28</v>
@@ -7304,7 +7308,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E94" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-29</v>
@@ -7346,7 +7350,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E95" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-30</v>
@@ -7388,7 +7392,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E96" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-03-31</v>
@@ -7433,7 +7437,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="97" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E97" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-01</v>
@@ -7478,7 +7482,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="98" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E98" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-02</v>
@@ -7523,7 +7527,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="99" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E99" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-03</v>
@@ -7565,7 +7569,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E100" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-04</v>
@@ -7607,7 +7611,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="101" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E101" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-05</v>
@@ -7649,7 +7653,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="102" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E102" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-06</v>
@@ -7691,7 +7695,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="103" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E103" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-07</v>
@@ -7733,7 +7737,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="104" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E104" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-08</v>
@@ -7775,7 +7779,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="105" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E105" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-09</v>
@@ -7817,7 +7821,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E106" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-10</v>
@@ -7859,7 +7863,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="107" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E107" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-11</v>
@@ -7901,7 +7905,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="108" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E108" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-12</v>
@@ -7943,7 +7947,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="109" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E109" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-13</v>
@@ -7985,7 +7989,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="110" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E110" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-14</v>
@@ -8027,7 +8031,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="111" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E111" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-15</v>
@@ -8069,7 +8073,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="112" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E112" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-16</v>
@@ -8111,7 +8115,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E113" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-17</v>
@@ -8153,7 +8157,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="114" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E114" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-18</v>
@@ -8195,7 +8199,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="115" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E115" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-19</v>
@@ -8237,7 +8241,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E116" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-20</v>
@@ -8279,7 +8283,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="117" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E117" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-21</v>
@@ -8321,7 +8325,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="118" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E118" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-22</v>
@@ -8363,7 +8367,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E119" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-23</v>
@@ -8405,7 +8409,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="120" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E120" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-24</v>
@@ -8447,7 +8451,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="121" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E121" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-25</v>
@@ -8489,7 +8493,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E122" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-26</v>
@@ -8531,7 +8535,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="123" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E123" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-27</v>
@@ -8573,7 +8577,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="124" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E124" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-28</v>
@@ -8615,7 +8619,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="125" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E125" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-29</v>
@@ -8657,7 +8661,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E126" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-04-30</v>
@@ -8699,7 +8703,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="127" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E127" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-01</v>
@@ -8741,7 +8745,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E128" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-02</v>
@@ -8783,7 +8787,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E129" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-03</v>
@@ -8825,7 +8829,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="130" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E130" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-04</v>
@@ -8867,7 +8871,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E131" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-05</v>
@@ -8909,7 +8913,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="132" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E132" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-06</v>
@@ -8951,7 +8955,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="133" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E133" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-07</v>
@@ -8993,7 +8997,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="134" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E134" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-08</v>
@@ -9035,7 +9039,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="135" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E135" s="1" t="d">
         <f t="shared" si="15"/>
         <v>2016-05-09</v>
@@ -9077,7 +9081,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="136" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E136" s="1" t="d">
         <f t="shared" ref="E136:E199" si="25">E135+1</f>
         <v>2016-05-10</v>
@@ -9119,7 +9123,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="137" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E137" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-11</v>
@@ -9161,7 +9165,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="138" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E138" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-12</v>
@@ -9203,7 +9207,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E139" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-13</v>
@@ -9245,7 +9249,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="140" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E140" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-14</v>
@@ -9287,7 +9291,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="141" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E141" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-15</v>
@@ -9329,7 +9333,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="142" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E142" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-16</v>
@@ -9371,7 +9375,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="143" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E143" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-17</v>
@@ -9413,7 +9417,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="144" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E144" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-18</v>
@@ -9455,7 +9459,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E145" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-19</v>
@@ -9497,7 +9501,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="146" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E146" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-20</v>
@@ -9539,7 +9543,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="147" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E147" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-21</v>
@@ -9581,7 +9585,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E148" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-22</v>
@@ -9623,7 +9627,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="149" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E149" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-23</v>
@@ -9665,7 +9669,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="150" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E150" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-24</v>
@@ -9707,7 +9711,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="151" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E151" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-25</v>
@@ -9749,7 +9753,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="152" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E152" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-26</v>
@@ -9791,7 +9795,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="153" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E153" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-27</v>
@@ -9833,7 +9837,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="154" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E154" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-28</v>
@@ -9875,7 +9879,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="155" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E155" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-29</v>
@@ -9917,7 +9921,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="156" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E156" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-30</v>
@@ -9959,7 +9963,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="157" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E157" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-05-31</v>
@@ -10001,7 +10005,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="158" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E158" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-01</v>
@@ -10043,7 +10047,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="159" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E159" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-02</v>
@@ -10085,7 +10089,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="160" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E160" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-03</v>
@@ -10127,7 +10131,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="161" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E161" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-04</v>
@@ -10169,7 +10173,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="162" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E162" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-05</v>
@@ -10211,7 +10215,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="163" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E163" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-06</v>
@@ -10253,7 +10257,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="164" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E164" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-07</v>
@@ -10295,7 +10299,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="165" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E165" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-08</v>
@@ -10337,7 +10341,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="166" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E166" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-09</v>
@@ -10379,7 +10383,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="167" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E167" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-10</v>
@@ -10421,7 +10425,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="168" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E168" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-11</v>
@@ -10463,7 +10467,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="169" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E169" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-12</v>
@@ -10505,7 +10509,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E170" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-13</v>
@@ -10547,7 +10551,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="171" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E171" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-14</v>
@@ -10589,7 +10593,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="172" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E172" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-15</v>
@@ -10631,7 +10635,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="173" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E173" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-16</v>
@@ -10673,7 +10677,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="174" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E174" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-17</v>
@@ -10715,7 +10719,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="175" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E175" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-18</v>
@@ -10757,7 +10761,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="176" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E176" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-19</v>
@@ -10799,7 +10803,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="177" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E177" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-20</v>
@@ -10841,7 +10845,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="178" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E178" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-21</v>
@@ -10883,7 +10887,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="179" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E179" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-22</v>
@@ -10925,7 +10929,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="180" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E180" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-23</v>
@@ -10967,7 +10971,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="181" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E181" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-24</v>
@@ -11009,7 +11013,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="182" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E182" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-25</v>
@@ -11051,7 +11055,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E183" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-26</v>
@@ -11093,7 +11097,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="184" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E184" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-27</v>
@@ -11135,7 +11139,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E185" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-28</v>
@@ -11177,7 +11181,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E186" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-29</v>
@@ -11219,7 +11223,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="187" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E187" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-06-30</v>
@@ -11261,7 +11265,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="188" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E188" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-01</v>
@@ -11303,7 +11307,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="189" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E189" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-02</v>
@@ -11345,7 +11349,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="190" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E190" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-03</v>
@@ -11387,7 +11391,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="191" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E191" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-04</v>
@@ -11429,7 +11433,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="192" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E192" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-05</v>
@@ -11471,7 +11475,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="193" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E193" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-06</v>
@@ -11513,7 +11517,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="194" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E194" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-07</v>
@@ -11555,7 +11559,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="195" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E195" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-08</v>
@@ -11597,7 +11601,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="196" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E196" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-09</v>
@@ -11639,7 +11643,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="197" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E197" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-10</v>
@@ -11681,7 +11685,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="198" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E198" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-11</v>
@@ -11723,7 +11727,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="199" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E199" s="1" t="d">
         <f t="shared" si="25"/>
         <v>2016-07-12</v>
@@ -11765,7 +11769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="200" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E200" s="1" t="d">
         <f t="shared" ref="E200:E263" si="35">E199+1</f>
         <v>2016-07-13</v>
@@ -11807,7 +11811,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="201" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E201" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-14</v>
@@ -11849,7 +11853,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="202" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E202" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-15</v>
@@ -11891,7 +11895,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="203" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E203" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-16</v>
@@ -11933,7 +11937,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="204" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E204" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-17</v>
@@ -11975,7 +11979,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="205" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E205" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-18</v>
@@ -12017,7 +12021,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="206" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E206" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-19</v>
@@ -12059,7 +12063,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="207" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E207" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-20</v>
@@ -12101,7 +12105,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="208" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E208" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-21</v>
@@ -12143,7 +12147,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="209" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E209" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-22</v>
@@ -12185,7 +12189,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="210" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E210" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-23</v>
@@ -12227,7 +12231,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="211" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E211" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-24</v>
@@ -12269,7 +12273,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="212" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E212" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-25</v>
@@ -12311,7 +12315,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="213" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E213" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-26</v>
@@ -12353,7 +12357,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="214" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E214" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-27</v>
@@ -12395,7 +12399,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="215" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E215" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-28</v>
@@ -12437,7 +12441,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="216" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E216" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-29</v>
@@ -12479,7 +12483,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="217" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E217" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-30</v>
@@ -12521,7 +12525,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="218" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E218" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-07-31</v>
@@ -12563,7 +12567,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="219" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E219" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-01</v>
@@ -12605,7 +12609,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="220" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="220" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E220" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-02</v>
@@ -12647,7 +12651,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="221" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="221" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E221" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-03</v>
@@ -12689,7 +12693,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="222" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="222" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E222" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-04</v>
@@ -12731,7 +12735,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="223" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="223" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E223" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-05</v>
@@ -12773,7 +12777,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="224" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="224" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E224" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-06</v>
@@ -12815,7 +12819,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="225" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="225" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E225" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-07</v>
@@ -12857,7 +12861,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="226" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="226" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E226" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-08</v>
@@ -12899,7 +12903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="227" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="227" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E227" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-09</v>
@@ -12941,7 +12945,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="228" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="228" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E228" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-10</v>
@@ -12983,7 +12987,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="229" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="229" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E229" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-11</v>
@@ -13025,7 +13029,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="230" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="230" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E230" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-12</v>
@@ -13067,7 +13071,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="231" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="231" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E231" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-13</v>
@@ -13109,7 +13113,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="232" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="232" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E232" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-14</v>
@@ -13151,7 +13155,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="233" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="233" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E233" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-15</v>
@@ -13193,7 +13197,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="234" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="234" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E234" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-16</v>
@@ -13235,7 +13239,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="235" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="235" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E235" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-17</v>
@@ -13277,7 +13281,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="236" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="236" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E236" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-18</v>
@@ -13319,7 +13323,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="237" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="237" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E237" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-19</v>
@@ -13361,7 +13365,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="238" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="238" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E238" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-20</v>
@@ -13403,7 +13407,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="239" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="239" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E239" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-21</v>
@@ -13445,7 +13449,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="240" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="240" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E240" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-22</v>
@@ -13487,7 +13491,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="241" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="241" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E241" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-23</v>
@@ -13529,7 +13533,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="242" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="242" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E242" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-24</v>
@@ -13571,7 +13575,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="243" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="243" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E243" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-25</v>
@@ -13613,7 +13617,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="244" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="244" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E244" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-26</v>
@@ -13655,7 +13659,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="245" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="245" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E245" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-27</v>
@@ -13697,7 +13701,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="246" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="246" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E246" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-28</v>
@@ -13739,7 +13743,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="247" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="247" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E247" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-29</v>
@@ -13781,7 +13785,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="248" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="248" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E248" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-30</v>
@@ -13823,7 +13827,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="249" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="249" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E249" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-08-31</v>
@@ -13865,7 +13869,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="250" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="250" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E250" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-01</v>
@@ -13907,7 +13911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="251" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="251" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E251" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-02</v>
@@ -13949,7 +13953,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="252" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="252" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E252" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-03</v>
@@ -13991,7 +13995,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="253" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="253" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E253" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-04</v>
@@ -14033,7 +14037,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="254" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="254" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E254" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-05</v>
@@ -14075,7 +14079,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="255" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="255" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E255" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-06</v>
@@ -14117,7 +14121,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="256" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="256" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E256" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-07</v>
@@ -14159,7 +14163,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="257" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="257" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E257" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-08</v>
@@ -14201,7 +14205,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="258" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="258" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E258" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-09</v>
@@ -14243,7 +14247,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="259" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="259" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E259" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-10</v>
@@ -14285,7 +14289,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="260" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="260" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E260" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-11</v>
@@ -14327,7 +14331,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="261" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="261" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E261" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-12</v>
@@ -14369,7 +14373,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="262" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="262" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E262" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-13</v>
@@ -14411,7 +14415,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="263" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="263" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E263" s="1" t="d">
         <f t="shared" si="35"/>
         <v>2016-09-14</v>
@@ -14453,7 +14457,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="264" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="264" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E264" s="1" t="d">
         <f t="shared" ref="E264:E327" si="45">E263+1</f>
         <v>2016-09-15</v>
@@ -14495,7 +14499,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="265" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="265" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E265" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-16</v>
@@ -14537,7 +14541,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="266" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="266" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E266" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-17</v>
@@ -14579,7 +14583,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="267" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="267" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E267" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-18</v>
@@ -14621,7 +14625,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="268" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="268" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E268" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-19</v>
@@ -14663,7 +14667,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="269" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="269" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E269" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-20</v>
@@ -14705,7 +14709,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="270" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="270" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E270" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-21</v>
@@ -14747,7 +14751,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="271" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="271" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E271" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-22</v>
@@ -14789,7 +14793,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="272" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="272" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E272" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-23</v>
@@ -14831,7 +14835,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="273" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="273" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E273" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-24</v>
@@ -14873,7 +14877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="274" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="274" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E274" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-25</v>
@@ -14915,7 +14919,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="275" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="275" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E275" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-26</v>
@@ -14957,7 +14961,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="276" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="276" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E276" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-27</v>
@@ -14999,7 +15003,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="277" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="277" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E277" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-28</v>
@@ -15041,7 +15045,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="278" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="278" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E278" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-29</v>
@@ -15083,7 +15087,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="279" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="279" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E279" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-09-30</v>
@@ -15125,7 +15129,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="280" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="280" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E280" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-01</v>
@@ -15167,7 +15171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="281" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="281" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E281" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-02</v>
@@ -15209,7 +15213,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="282" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="282" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E282" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-03</v>
@@ -15251,7 +15255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="283" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="283" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E283" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-04</v>
@@ -15293,7 +15297,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="284" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="284" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E284" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-05</v>
@@ -15335,7 +15339,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="285" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="285" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E285" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-06</v>
@@ -15377,7 +15381,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="286" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="286" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E286" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-07</v>
@@ -15419,7 +15423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="287" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="287" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E287" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-08</v>
@@ -15461,7 +15465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="288" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="288" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E288" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-09</v>
@@ -15503,7 +15507,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="289" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="289" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E289" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-10</v>
@@ -15545,7 +15549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="290" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="290" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E290" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-11</v>
@@ -15587,7 +15591,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="291" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="291" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E291" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-12</v>
@@ -15629,7 +15633,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="292" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E292" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-13</v>
@@ -15671,7 +15675,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="293" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="293" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E293" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-14</v>
@@ -15713,7 +15717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="294" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="294" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E294" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-15</v>
@@ -15755,7 +15759,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="295" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="295" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E295" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-16</v>
@@ -15797,7 +15801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="296" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="296" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E296" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-17</v>
@@ -15839,7 +15843,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="297" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="297" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E297" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-18</v>
@@ -15881,7 +15885,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="298" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="298" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E298" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-19</v>
@@ -15923,7 +15927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="299" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="299" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E299" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-20</v>
@@ -15965,7 +15969,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="300" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="300" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E300" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-21</v>
@@ -16007,7 +16011,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="301" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="301" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E301" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-22</v>
@@ -16049,7 +16053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="302" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="302" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E302" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-23</v>
@@ -16091,7 +16095,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="303" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="303" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E303" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-24</v>
@@ -16133,7 +16137,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="304" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="304" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E304" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-25</v>
@@ -16175,7 +16179,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="305" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="305" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E305" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-26</v>
@@ -16217,7 +16221,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="306" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="306" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E306" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-27</v>
@@ -16259,7 +16263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="307" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="307" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E307" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-28</v>
@@ -16301,7 +16305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="308" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="308" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E308" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-29</v>
@@ -16343,7 +16347,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="309" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="309" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E309" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-30</v>
@@ -16385,7 +16389,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="310" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="310" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E310" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-10-31</v>
@@ -16427,7 +16431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="311" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="311" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E311" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-01</v>
@@ -16469,7 +16473,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="312" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="312" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E312" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-02</v>
@@ -16511,7 +16515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="313" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="313" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E313" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-03</v>
@@ -16553,7 +16557,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="314" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="314" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E314" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-04</v>
@@ -16595,7 +16599,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="315" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="315" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E315" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-05</v>
@@ -16637,7 +16641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="316" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="316" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E316" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-06</v>
@@ -16679,7 +16683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="317" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="317" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E317" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-07</v>
@@ -16721,7 +16725,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="318" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="318" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E318" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-08</v>
@@ -16763,7 +16767,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="319" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="319" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E319" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-09</v>
@@ -16805,7 +16809,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="320" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="320" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E320" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-10</v>
@@ -16847,7 +16851,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="321" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="321" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E321" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-11</v>
@@ -16889,7 +16893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="322" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="322" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E322" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-12</v>
@@ -16931,7 +16935,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="323" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="323" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E323" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-13</v>
@@ -16973,7 +16977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="324" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="324" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E324" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-14</v>
@@ -17015,7 +17019,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="325" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="325" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E325" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-15</v>
@@ -17057,7 +17061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="326" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="326" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E326" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-16</v>
@@ -17099,7 +17103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="327" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="327" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E327" s="1" t="d">
         <f t="shared" si="45"/>
         <v>2016-11-17</v>
@@ -17141,7 +17145,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="328" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="328" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E328" s="1" t="d">
         <f t="shared" ref="E328:E371" si="55">E327+1</f>
         <v>2016-11-18</v>
@@ -17183,7 +17187,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="329" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="329" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E329" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-19</v>
@@ -17225,7 +17229,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="330" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="330" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E330" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-20</v>
@@ -17267,7 +17271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="331" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="331" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E331" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-21</v>
@@ -17309,7 +17313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="332" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="332" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E332" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-22</v>
@@ -17351,7 +17355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="333" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="333" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E333" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-23</v>
@@ -17393,7 +17397,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="334" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="334" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E334" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-24</v>
@@ -17435,7 +17439,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="335" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="335" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E335" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-25</v>
@@ -17477,7 +17481,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="336" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="336" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E336" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-26</v>
@@ -17519,7 +17523,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="337" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="337" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E337" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-27</v>
@@ -17561,7 +17565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="338" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="338" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E338" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-28</v>
@@ -17603,7 +17607,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="339" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="339" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E339" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-29</v>
@@ -17645,7 +17649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="340" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="340" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E340" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-11-30</v>
@@ -17687,7 +17691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="341" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="341" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E341" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-01</v>
@@ -17729,7 +17733,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="342" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="342" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E342" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-02</v>
@@ -17771,7 +17775,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="343" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="343" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E343" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-03</v>
@@ -17813,7 +17817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="344" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="344" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E344" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-04</v>
@@ -17855,7 +17859,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="345" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="345" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E345" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-05</v>
@@ -17897,7 +17901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="346" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="346" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E346" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-06</v>
@@ -17939,7 +17943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="347" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="347" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E347" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-07</v>
@@ -17981,7 +17985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="348" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="348" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E348" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-08</v>
@@ -18023,7 +18027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="349" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="349" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E349" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-09</v>
@@ -18065,7 +18069,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="350" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="350" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E350" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-10</v>
@@ -18107,7 +18111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="351" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="351" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E351" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-11</v>
@@ -18149,7 +18153,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="352" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="352" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E352" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-12</v>
@@ -18191,7 +18195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="353" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="353" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E353" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-13</v>
@@ -18233,7 +18237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="354" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="354" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E354" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-14</v>
@@ -18275,7 +18279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="355" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="355" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E355" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-15</v>
@@ -18317,7 +18321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="356" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="356" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E356" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-16</v>
@@ -18359,7 +18363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="357" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E357" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-17</v>
@@ -18401,7 +18405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="358" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="358" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E358" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-18</v>
@@ -18443,7 +18447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="359" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="359" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E359" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-19</v>
@@ -18485,7 +18489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="360" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="360" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E360" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-20</v>
@@ -18527,7 +18531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="361" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="361" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E361" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-21</v>
@@ -18569,7 +18573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="362" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="362" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E362" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-22</v>
@@ -18611,7 +18615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="363" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="363" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E363" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-23</v>
@@ -18653,7 +18657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="364" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="364" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E364" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-24</v>
@@ -18695,7 +18699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="365" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="365" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E365" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-25</v>
@@ -18737,7 +18741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="366" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="366" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E366" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-26</v>
@@ -18782,7 +18786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="367" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="367" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E367" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-27</v>
@@ -18827,7 +18831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="368" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E368" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-28</v>
@@ -18872,7 +18876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="369" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E369" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-29</v>
@@ -18917,7 +18921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="370" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E370" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-30</v>
@@ -18962,7 +18966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="371" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E371" s="1" t="d">
         <f t="shared" si="55"/>
         <v>2016-12-31</v>

</xml_diff>